<commit_message>
ALL FOREIGN KEY working
</commit_message>
<xml_diff>
--- a/kochrezept_datenmodell.xlsx
+++ b/kochrezept_datenmodell.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\iCloud\projects\database\kochrezept\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4C2A12-305C-473F-A723-F29CCBBCDE9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A87525-E008-4643-BFFA-FFDEF4EF3FA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>rezept</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>rezept_kategorie_beschreibung</t>
+  </si>
+  <si>
+    <t>rezept_portionen</t>
+  </si>
+  <si>
+    <t>zutat_kategorie_beschreibung</t>
   </si>
 </sst>
 </file>
@@ -348,7 +354,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-            <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+            <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -455,15 +461,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>348028</xdr:colOff>
+      <xdr:colOff>335816</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>161290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2033341</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>154689</xdr:rowOff>
+      <xdr:colOff>2021129</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>148584</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -475,14 +481,13 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="49" idx="3"/>
           <a:endCxn id="53" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4200769" y="1877012"/>
-          <a:ext cx="1685313" cy="1312245"/>
+          <a:off x="4188557" y="1877012"/>
+          <a:ext cx="1685313" cy="1605322"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -520,13 +525,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>177067</xdr:colOff>
+      <xdr:colOff>170961</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>161289</xdr:rowOff>
+      <xdr:rowOff>152643</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2033373</xdr:colOff>
+      <xdr:colOff>1966057</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>163695</xdr:rowOff>
     </xdr:to>
@@ -539,15 +544,12 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="55" idx="3"/>
-          <a:endCxn id="57" idx="1"/>
-        </xdr:cNvCxnSpPr>
+        <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8523654" y="1877011"/>
-          <a:ext cx="1856306" cy="2406"/>
+          <a:off x="8517548" y="1868365"/>
+          <a:ext cx="1795096" cy="11052"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -585,15 +587,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>226054</xdr:colOff>
+      <xdr:colOff>256442</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>161288</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2053491</xdr:colOff>
+      <xdr:colOff>2029068</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>179721</xdr:rowOff>
+      <xdr:rowOff>170962</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -604,15 +606,12 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="60" idx="1"/>
-          <a:endCxn id="58" idx="3"/>
-        </xdr:cNvCxnSpPr>
+        <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="13066487" y="1877010"/>
-          <a:ext cx="1827437" cy="366461"/>
+          <a:off x="13096875" y="1877010"/>
+          <a:ext cx="1772626" cy="357702"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -652,13 +651,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>235584</xdr:colOff>
+      <xdr:colOff>217266</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>161288</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
+      <xdr:colOff>934182</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>160793</xdr:rowOff>
     </xdr:to>
@@ -671,14 +670,11 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="62" idx="1"/>
-          <a:endCxn id="63" idx="3"/>
-        </xdr:cNvCxnSpPr>
+        <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="17496594" y="1877010"/>
+          <a:off x="17478276" y="1877010"/>
           <a:ext cx="1840378" cy="1318351"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
@@ -721,13 +717,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>226054</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>166178</xdr:rowOff>
+      <xdr:rowOff>153968</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2053491</xdr:colOff>
+      <xdr:colOff>2102339</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>70804</xdr:rowOff>
+      <xdr:rowOff>70803</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -745,8 +741,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="13066487" y="2565746"/>
-          <a:ext cx="1827437" cy="1882895"/>
+          <a:off x="13066487" y="2553536"/>
+          <a:ext cx="1876285" cy="1895104"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -880,9 +876,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2033341</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>21607</xdr:rowOff>
+      <xdr:colOff>2021129</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>15502</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="212751" cy="266163"/>
     <xdr:sp macro="" textlink="">
@@ -898,7 +894,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5886082" y="3056175"/>
+          <a:off x="5873870" y="3349252"/>
           <a:ext cx="212751" cy="266163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1276,7 +1272,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>13302</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>33095</xdr:rowOff>
+      <xdr:rowOff>20886</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="212751" cy="266163"/>
     <xdr:sp macro="" textlink="">
@@ -1292,7 +1288,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12853735" y="2432663"/>
+          <a:off x="12853735" y="2420454"/>
           <a:ext cx="212751" cy="266163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1474,7 +1470,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2053490</xdr:colOff>
+      <xdr:colOff>2102338</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>285750</xdr:rowOff>
     </xdr:from>
@@ -1492,7 +1488,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14893923" y="4315558"/>
+          <a:off x="14942771" y="4315558"/>
           <a:ext cx="173124" cy="266163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2852,18 +2848,18 @@
   <dimension ref="B1:K31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="78" zoomScaleNormal="100" zoomScalePageLayoutView="78" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.46484375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="38.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.9296875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="39.9296875" style="5" customWidth="1"/>
     <col min="3" max="6" width="32.59765625" style="5" customWidth="1"/>
     <col min="7" max="7" width="33.19921875" style="5" customWidth="1"/>
     <col min="8" max="8" width="30.86328125" style="5" customWidth="1"/>
     <col min="9" max="10" width="16.33203125" style="5"/>
-    <col min="11" max="11" width="28.06640625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="42.53125" style="5" customWidth="1"/>
     <col min="12" max="16384" width="16.33203125" style="5"/>
   </cols>
   <sheetData>
@@ -2932,6 +2928,9 @@
       <c r="H5" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="K5" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="2:11" ht="23.65">
       <c r="D6" s="3" t="s">
@@ -2945,11 +2944,16 @@
       </c>
     </row>
     <row r="7" spans="2:11" ht="23.65">
-      <c r="D7" s="7" t="s">
-        <v>5</v>
+      <c r="D7" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="19.899999999999999" customHeight="1">
+      <c r="D8" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="35.450000000000003" customHeight="1"/>
@@ -2992,7 +2996,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.74803149606299213" bottom="0.74803149606299213" header="0.27559055118110237" footer="0.27559055118110237"/>
-  <pageSetup scale="42" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="40" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Gill Sans MT,Standard"&amp;16DATENMODELL - Kochrezept</oddHeader>
     <oddFooter>&amp;R&amp;"Helvetica Neue,Fett"2020 // heiko mlodystach // veaceslav  pintea</oddFooter>

</xml_diff>